<commit_message>
Ran scraper for Australia and added excel files
</commit_message>
<xml_diff>
--- a/bin/sheets/main_db/utility/PureBatsmen_ODI.xlsx
+++ b/bin/sheets/main_db/utility/PureBatsmen_ODI.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,105 +436,70 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>AUS</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>3832</t>
+          <t>4369</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>4931</t>
+          <t>4726</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>4544</t>
+          <t>4558</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3210</t>
+          <t>6471</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>4083</t>
+          <t>3842</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4542</t>
+          <t>4824</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>3826</t>
+          <t>3725</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>3889</t>
+          <t>5860</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4137</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>3759</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>4099</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>4759</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>4769</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>4073</t>
+          <t>3910</t>
         </is>
       </c>
     </row>

</xml_diff>